<commit_message>
Updating output job file and BOM template
Changing output job file .pdf outputs from mono to colour. Updating BOM template to refer to the correct parameters for PCB details i.e. PCBName, PCBDesigner etc.
</commit_message>
<xml_diff>
--- a/Shared Libraries/APSSTemplates/APSS BOM Template.xlsx
+++ b/Shared Libraries/APSSTemplates/APSS BOM Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vontier-my.sharepoint.com/personal/filipk_invenco_com/Documents/Documents/APSS-Reference-PCBs/Shared Libraries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vontier-my.sharepoint.com/personal/filipk_invenco_com/Documents/Documents/APSS-Reference-PCBs/Shared Libraries/APSSTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{BB9DF1E4-5EE3-4857-84AF-92CD1321BAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E606942-CEB7-4AF8-A26B-05FCD0F64A88}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{BB9DF1E4-5EE3-4857-84AF-92CD1321BAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BAD957D-C698-47C9-87C8-56CBFF4EED60}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{8143E680-549F-46F0-B77E-A70799F379B4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8143E680-549F-46F0-B77E-A70799F379B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,13 +92,13 @@
     <t>Field=Project</t>
   </si>
   <si>
-    <t>Field=PCBName</t>
-  </si>
-  <si>
-    <t>Field=PCBRevision</t>
-  </si>
-  <si>
-    <t>Field=PCBDesigner</t>
+    <t>Field=DesignName</t>
+  </si>
+  <si>
+    <t>Field=BoardRevision</t>
+  </si>
+  <si>
+    <t>Field=Designer</t>
   </si>
 </sst>
 </file>
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B358C88E-7CF8-41D0-B20D-DBF0AE37A859}">
   <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Adding Board Outline mech layer to PCB/Outjob Template
Adding a mechanical layer 5 named 'Board Outline' to the PCB template. Adding Mech Layer 5 to be exported as a gerber in the outjob file template.
</commit_message>
<xml_diff>
--- a/Shared Libraries/APSSTemplates/APSS BOM Template.xlsx
+++ b/Shared Libraries/APSSTemplates/APSS BOM Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vontier-my.sharepoint.com/personal/filipk_invenco_com/Documents/Documents/APSS-Reference-PCBs/Shared Libraries/APSSTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{BB9DF1E4-5EE3-4857-84AF-92CD1321BAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BAD957D-C698-47C9-87C8-56CBFF4EED60}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE781ED5-DEC3-4432-A6B6-20D209397375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8143E680-549F-46F0-B77E-A70799F379B4}"/>
+    <workbookView xWindow="1365" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{8143E680-549F-46F0-B77E-A70799F379B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>PCB Name:</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Field=Designer</t>
+  </si>
+  <si>
+    <t>Column=APSS Standard Part</t>
   </si>
 </sst>
 </file>
@@ -630,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B358C88E-7CF8-41D0-B20D-DBF0AE37A859}">
-  <dimension ref="B2:I13"/>
+  <dimension ref="B2:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,10 +648,11 @@
     <col min="6" max="6" width="16.7265625" customWidth="1"/>
     <col min="7" max="7" width="16.26953125" customWidth="1"/>
     <col min="8" max="8" width="38.36328125" customWidth="1"/>
-    <col min="9" max="9" width="10.6328125" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" customWidth="1"/>
+    <col min="10" max="10" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7" t="s">
@@ -656,7 +660,7 @@
       </c>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="1" t="s">
@@ -666,7 +670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="1" t="s">
@@ -676,7 +680,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="1" t="s">
@@ -686,7 +690,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="1" t="s">
@@ -696,7 +700,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="1" t="s">
@@ -706,7 +710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="1" t="s">
@@ -716,7 +720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -739,10 +743,13 @@
         <v>15</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -751,8 +758,9 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -761,8 +769,9 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -771,6 +780,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>